<commit_message>
updates to LCOM model and LCOA data
</commit_message>
<xml_diff>
--- a/LCOA_PyPSA_results.xlsx
+++ b/LCOA_PyPSA_results.xlsx
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="25" t="n"/>
+      <c r="A3" s="27" t="n"/>
       <c r="B3" s="25" t="inlineStr">
         <is>
           <t>wind</t>
@@ -3253,7 +3253,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="25" t="n"/>
+      <c r="A5" s="28" t="n"/>
       <c r="B5" s="25" t="inlineStr">
         <is>
           <t>Haber-Bosch</t>
@@ -3297,7 +3297,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="25" t="n"/>
+      <c r="A6" s="28" t="n"/>
       <c r="B6" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
@@ -3341,7 +3341,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="n"/>
+      <c r="A7" s="27" t="n"/>
       <c r="B7" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
@@ -3413,7 +3413,6 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>0</v>
       </c>
@@ -3426,7 +3425,6 @@
       <c r="M8" t="n">
         <v>-106400833.7040003</v>
       </c>
-      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="25" t="inlineStr">
@@ -3525,7 +3523,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="25" t="n"/>
+      <c r="A11" s="27" t="n"/>
       <c r="B11" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
@@ -4310,84 +4308,84 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>498.06036</v>
+        <v>491.0377</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>641301.0951105601</v>
+        <v>632556.61968711</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>641301.0951105601</v>
+        <v>632556.61968711</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1469859748920766</v>
+        <v>0.147055225661153</v>
       </c>
       <c r="J2" t="n">
-        <v>181502.4422655519</v>
+        <v>178645.37256398</v>
       </c>
       <c r="K2" t="n">
-        <v>23706074.81012189</v>
+        <v>23371818.73054541</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>23706074.9508638</v>
+        <v>23371818.7324545</v>
       </c>
       <c r="N2" t="n">
-        <v>36.96559249875737</v>
+        <v>36.94818456569977</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="27" t="n"/>
+      <c r="A3" s="25" t="n"/>
       <c r="B3" s="25" t="inlineStr">
         <is>
           <t>wind</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>473.27868</v>
+        <v>466.76337</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1324724.022055071</v>
+        <v>1306077.962209599</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1324724.022055071</v>
+        <v>1306077.962209599</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3195246475732738</v>
+        <v>0.3194245036547839</v>
       </c>
       <c r="J3" t="n">
-        <v>272183.08545635</v>
+        <v>268845.5981083991</v>
       </c>
       <c r="K3" t="n">
-        <v>31471807.81468588</v>
+        <v>31038556.55525222</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>31471807.54236151</v>
+        <v>31038556.53982739</v>
       </c>
       <c r="N3" t="n">
-        <v>23.75725586491491</v>
+        <v>23.76470428098861</v>
       </c>
     </row>
     <row r="4">
@@ -4402,113 +4400,113 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>297.06287</v>
+        <v>296.05771</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1068290.751890159</v>
+        <v>1068290.758459571</v>
       </c>
       <c r="F4" t="n">
-        <v>1810662.291339254</v>
+        <v>1810662.302473841</v>
       </c>
       <c r="G4" t="n">
-        <v>-742371.539449095</v>
+        <v>-742371.5440142702</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6958008875372803</v>
+        <v>0.6981632394287055</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>26031750.61403696</v>
+        <v>25943667.99890837</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>26031751.47735161</v>
+        <v>25943667.8071617</v>
       </c>
       <c r="N4" t="n">
-        <v>24.36766529270492</v>
+        <v>24.28521224368868</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="28" t="n"/>
+      <c r="A5" s="25" t="n"/>
       <c r="B5" s="25" t="inlineStr">
         <is>
           <t>Haber-Bosch</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>131.70442</v>
+        <v>131.70582</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>876000.0207935935</v>
+        <v>876000.0183557372</v>
       </c>
       <c r="F5" t="n">
-        <v>1219988.076878838</v>
+        <v>1192682.784991522</v>
       </c>
       <c r="G5" t="n">
-        <v>-343988.0560852446</v>
+        <v>-316682.7666357846</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9259446485907528</v>
+        <v>0.9259348034533702</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>9902271.079181343</v>
+        <v>9902376.338970732</v>
       </c>
       <c r="L5" t="n">
-        <v>11592023.31191969</v>
+        <v>11592023.27965964</v>
       </c>
       <c r="M5" t="n">
-        <v>21494293.60706124</v>
+        <v>21494398.50771629</v>
       </c>
       <c r="N5" t="n">
-        <v>24.53686426581334</v>
+        <v>24.53698408369945</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="28" t="n"/>
+      <c r="A6" s="25" t="n"/>
       <c r="B6" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>35.201311</v>
+        <v>35.200622</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>108450.6840391261</v>
+        <v>108404.7157789306</v>
       </c>
       <c r="F6" t="n">
-        <v>108450.6840391261</v>
+        <v>108404.7157789306</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.000497146655106917</v>
+        <v>-0.0009200225285894703</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3516975567461</v>
+        <v>0.3515553661146246</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -4517,42 +4515,42 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0004971458420186536</v>
+        <v>-0.0009200232925650198</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0004971693269908428</v>
+        <v>-0.0009200111962854862</v>
       </c>
       <c r="N6" t="n">
-        <v>-4.584383412373058e-09</v>
+        <v>-8.486806698009722e-09</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="27" t="n"/>
+      <c r="A7" s="25" t="n"/>
       <c r="B7" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>131.70442</v>
+        <v>131.70582</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>368680.8248146373</v>
+        <v>364178.8738114332</v>
       </c>
       <c r="F7" t="n">
-        <v>368680.8248146373</v>
+        <v>364178.8738114332</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.001196602773461564</v>
+        <v>-5.214291513766511e-05</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3195553508970281</v>
+        <v>0.3156499143347808</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -4561,13 +4559,13 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.001196602857589824</v>
+        <v>-5.214296629674209e-05</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.001196608878672123</v>
+        <v>-5.222856998443604e-05</v>
       </c>
       <c r="N7" t="n">
-        <v>-3.245536016387065e-09</v>
+        <v>-1.431855466646022e-10</v>
       </c>
     </row>
     <row r="8">
@@ -4599,6 +4597,7 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
         <v>0</v>
       </c>
@@ -4609,8 +4608,9 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>-115586113.5558973</v>
-      </c>
+        <v>-114583742.4676979</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="25" t="inlineStr">
@@ -4624,40 +4624,40 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>91.33242300000001</v>
+        <v>89.74455</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>49631.82455070817</v>
+        <v>48477.60845142997</v>
       </c>
       <c r="F9" t="n">
-        <v>53297.34978118995</v>
+        <v>52057.88979522099</v>
       </c>
       <c r="G9" t="n">
-        <v>-3665.525230481805</v>
+        <v>-3580.281343791002</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1286498853276944</v>
+        <v>0.1278813593804588</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1878799.835008928</v>
+        <v>1846135.689764307</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>1878799.844273967</v>
+        <v>1846135.699611556</v>
       </c>
       <c r="N9" t="n">
-        <v>37.8547406081036</v>
+        <v>38.0822354605469</v>
       </c>
     </row>
     <row r="10">
@@ -4672,84 +4672,84 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>25460.487</v>
+        <v>25462.197</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>54225.34226813618</v>
+        <v>54202.35834947717</v>
       </c>
       <c r="F10" t="n">
-        <v>54225.34177098911</v>
+        <v>54202.35742945455</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000497146655106917</v>
+        <v>0.0009200225285894703</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4277554526197086</v>
+        <v>0.4276846945636308</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2900667.462340149</v>
+        <v>2900862.27956264</v>
       </c>
       <c r="L10" t="n">
-        <v>0.000497146655106917</v>
+        <v>0.0009200225285894703</v>
       </c>
       <c r="M10" t="n">
-        <v>2900667.570487224</v>
+        <v>2900862.315955255</v>
       </c>
       <c r="N10" t="n">
-        <v>53.49284023222694</v>
+        <v>53.5191162209516</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="27" t="n"/>
+      <c r="A11" s="25" t="n"/>
       <c r="B11" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5064.4683</v>
+        <v>4992.9548</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>184340.4130056199</v>
+        <v>182089.4369317884</v>
       </c>
       <c r="F11" t="n">
-        <v>184340.4118090167</v>
+        <v>182089.4368796445</v>
       </c>
       <c r="G11" t="n">
-        <v>0.001196602763911869</v>
+        <v>5.214291718402819e-05</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2912016108879386</v>
+        <v>0.2912925344744648</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>8102719.615922358</v>
+        <v>7988304.083051263</v>
       </c>
       <c r="L11" t="n">
-        <v>0.001196602763911869</v>
+        <v>5.214291718402819e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>8102719.555755445</v>
+        <v>7988303.936623202</v>
       </c>
       <c r="N11" t="n">
-        <v>43.95519909955109</v>
+        <v>43.87022153083839</v>
       </c>
     </row>
     <row r="14">
@@ -4771,7 +4771,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>876000.0207935935</v>
+        <v>876000.0183557372</v>
       </c>
     </row>
     <row r="16">
@@ -4781,7 +4781,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>103994091.2312975</v>
+        <v>102991721.6760549</v>
       </c>
     </row>
     <row r="17">
@@ -4791,7 +4791,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>11592023.31191969</v>
+        <v>11592023.27965964</v>
       </c>
     </row>
     <row r="18">
@@ -4801,7 +4801,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>686.1276042895788</v>
+        <v>680.1774672198139</v>
       </c>
     </row>
   </sheetData>
@@ -5421,278 +5421,278 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="25" t="inlineStr">
         <is>
           <t>Optimal Capacity</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="25" t="inlineStr">
         <is>
           <t>Installed Capacity</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="25" t="inlineStr">
         <is>
           <t>Supply</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="25" t="inlineStr">
         <is>
           <t>Withdrawal</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Energy Balance</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="G1" s="25" t="inlineStr">
+        <is>
+          <t>Dispatch</t>
+        </is>
+      </c>
+      <c r="H1" s="25" t="inlineStr">
         <is>
           <t>Transmission</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="25" t="inlineStr">
         <is>
           <t>Capacity Factor</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="25" t="inlineStr">
         <is>
           <t>Curtailment</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="25" t="inlineStr">
         <is>
           <t>Capital Expenditure</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="25" t="inlineStr">
         <is>
           <t>Operational Expenditure</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="25" t="inlineStr">
         <is>
           <t>Revenue</t>
         </is>
       </c>
-      <c r="N1" s="3" t="inlineStr">
+      <c r="N1" s="25" t="inlineStr">
         <is>
           <t>Market Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="24" t="inlineStr">
+      <c r="A2" s="26" t="inlineStr">
         <is>
           <t>Generator</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>solar</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>400.52243</v>
+        <v>466.17442</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>407214.13289</v>
+        <v>562647.4985286598</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>407214.13289</v>
+        <v>562647.4985286598</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1160624886850906</v>
+        <v>0.1377792597429637</v>
       </c>
       <c r="J2" t="n">
-        <v>258056.79061</v>
+        <v>211671.8989970179</v>
       </c>
       <c r="K2" t="n">
-        <v>17002206.19579</v>
+        <v>22188406.39131606</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>17002206.34174</v>
+        <v>22188406.5317782</v>
       </c>
       <c r="N2" t="n">
-        <v>41.75249706199529</v>
+        <v>39.43571523876238</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="n"/>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="A3" s="27" t="n"/>
+      <c r="B3" s="25" t="inlineStr">
         <is>
           <t>wind</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>999.53217</v>
+        <v>467.1495</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1529125.44776</v>
+        <v>1374654.249352331</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1529125.44776</v>
+        <v>1374654.249352331</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1746394015512277</v>
+        <v>0.3359181612473474</v>
       </c>
       <c r="J3" t="n">
-        <v>2217098.13867</v>
+        <v>376211.3346121699</v>
       </c>
       <c r="K3" t="n">
-        <v>54830832.66655</v>
+        <v>31064233.20130668</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>54830833.05919</v>
+        <v>31064233.09717453</v>
       </c>
       <c r="N3" t="n">
-        <v>35.85764202896807</v>
+        <v>22.59785186843196</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24" t="inlineStr">
+      <c r="A4" s="26" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Electrolyser</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>309.66186</v>
+        <v>298.99591</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1068290.75286</v>
+        <v>1068290.757641756</v>
       </c>
       <c r="F4" t="n">
-        <v>1810662.29298</v>
+        <v>1810662.301087716</v>
       </c>
       <c r="G4" t="n">
-        <v>-742371.54012</v>
+        <v>-742371.5434459604</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6674913403930338</v>
+        <v>0.6913024653521518</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>16038889.36289</v>
+        <v>26201143.76373271</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>16038888.21619</v>
+        <v>26201144.61798178</v>
       </c>
       <c r="N4" t="n">
-        <v>15.0135981664767</v>
+        <v>24.52622980266229</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="20" t="n"/>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="A5" s="28" t="n"/>
+      <c r="B5" s="25" t="inlineStr">
         <is>
           <t>Haber-Bosch</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14.46797</v>
+        <v>131.28506</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>875999.99341</v>
+        <v>876000.0090151001</v>
       </c>
       <c r="F5" t="n">
-        <v>1192682.75103</v>
+        <v>1192682.772274148</v>
       </c>
       <c r="G5" t="n">
-        <v>-316682.75762</v>
+        <v>-316682.7632590476</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9814783967619507</v>
+        <v>0.928902353817135</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>6319415.50454</v>
+        <v>9870741.261125384</v>
       </c>
       <c r="L5" t="n">
-        <v>9505475.928479999</v>
+        <v>11592023.15605588</v>
       </c>
       <c r="M5" t="n">
-        <v>15824891.9032</v>
+        <v>21462765.02196079</v>
       </c>
       <c r="N5" t="n">
-        <v>18.0649451</v>
+        <v>24.50087306059726</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="n"/>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="A6" s="28" t="n"/>
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>38.86775</v>
+        <v>35.407635</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>30946.00507</v>
+        <v>104835.3080856641</v>
       </c>
       <c r="F6" t="n">
-        <v>30946.00507</v>
+        <v>104835.3080856641</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.00035</v>
+        <v>-0.0002678043592823087</v>
       </c>
       <c r="I6" t="n">
-        <v>0.09088897607914015</v>
+        <v>0.3379921003766856</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -5701,39 +5701,42 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.00035</v>
+        <v>-0.0002678038808880956</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.00035</v>
+        <v>-0.0002678781747817993</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-2.554897145309511e-09</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="n"/>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="A7" s="27" t="n"/>
+      <c r="B7" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>124.25232</v>
+        <v>131.28506</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>330420.41102</v>
+        <v>353931.3764863742</v>
       </c>
       <c r="F7" t="n">
-        <v>330420.41102</v>
+        <v>353931.3764863742</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.00072</v>
+        <v>0.001078938296302567</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3035696234887204</v>
+        <v>0.3077511269726921</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -5742,19 +5745,22 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.00072</v>
+        <v>0.001078938273337826</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.00072</v>
+        <v>0.001078936271369457</v>
+      </c>
+      <c r="N7" t="n">
+        <v>3.048439953121049e-09</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="25" t="inlineStr">
         <is>
           <t>Load</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5787,156 +5793,156 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>-115798398.6337</v>
+        <v>-111219098.959199</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="25" t="inlineStr">
         <is>
           <t>StorageUnit</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>68.11892</v>
+        <v>66.63944100000001</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>17402.76722</v>
+        <v>30430.76019861499</v>
       </c>
       <c r="F9" t="n">
-        <v>18688.03691</v>
+        <v>32678.20368023996</v>
       </c>
       <c r="G9" t="n">
-        <v>-1285.2697</v>
+        <v>-2247.443481625</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.06048172813074547</v>
+        <v>0.1081074437715325</v>
       </c>
       <c r="J9" t="n">
-        <v>598007.0089</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1256356.1538</v>
+        <v>1370840.350484156</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>1256356.16246</v>
+        <v>1370840.348979826</v>
       </c>
       <c r="N9" t="n">
-        <v>72.19279479719322</v>
+        <v>45.04785092559786</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="24" t="inlineStr">
+      <c r="A10" s="26" t="inlineStr">
         <is>
           <t>Store</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7431.342</v>
+        <v>28286.994</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>15473.00271</v>
+        <v>52417.65417673375</v>
       </c>
       <c r="F10" t="n">
-        <v>15473.00236</v>
+        <v>52417.65390892929</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00035</v>
+        <v>0.0002678043592823087</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3551887559474453</v>
+        <v>0.4098789215709231</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>71612.29736</v>
+        <v>3222686.317948711</v>
       </c>
       <c r="L10" t="n">
-        <v>0.00035</v>
+        <v>0.0002678043592823087</v>
       </c>
       <c r="M10" t="n">
-        <v>71612.33189</v>
+        <v>3222686.502660474</v>
       </c>
       <c r="N10" t="n">
-        <v>4.628221386838172</v>
+        <v>61.48093716278913</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="n"/>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="A11" s="27" t="n"/>
+      <c r="B11" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2124.3904</v>
+        <v>3568.3288</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>165210.20587</v>
+        <v>176965.687703718</v>
       </c>
       <c r="F11" t="n">
-        <v>165210.20515</v>
+        <v>176965.6887826571</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00072</v>
+        <v>-0.001078938299940546</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1394292357939482</v>
+        <v>0.2889678274382066</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>10773609.86819</v>
+        <v>5709023.346798455</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00072</v>
+        <v>-0.001078938299940546</v>
       </c>
       <c r="M11" t="n">
-        <v>10773610.03898</v>
+        <v>5709023.189771163</v>
       </c>
       <c r="N11" t="n">
-        <v>65.21153724811913</v>
+        <v>32.26062217964775</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="25" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="25" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -5949,7 +5955,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>875999.99341</v>
+        <v>876000.0090151001</v>
       </c>
     </row>
     <row r="16">
@@ -5959,7 +5965,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>106292922.04912</v>
+        <v>99627074.63271216</v>
       </c>
     </row>
     <row r="17">
@@ -5969,7 +5975,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9505475.928479999</v>
+        <v>11592023.15605587</v>
       </c>
     </row>
     <row r="18">
@@ -5979,7 +5985,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>687.3877557230655</v>
+        <v>660.2046832760075</v>
       </c>
     </row>
   </sheetData>
@@ -6007,278 +6013,278 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="25" t="inlineStr">
         <is>
           <t>Optimal Capacity</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="25" t="inlineStr">
         <is>
           <t>Installed Capacity</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="25" t="inlineStr">
         <is>
           <t>Supply</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="25" t="inlineStr">
         <is>
           <t>Withdrawal</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Energy Balance</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="G1" s="25" t="inlineStr">
+        <is>
+          <t>Dispatch</t>
+        </is>
+      </c>
+      <c r="H1" s="25" t="inlineStr">
         <is>
           <t>Transmission</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="25" t="inlineStr">
         <is>
           <t>Capacity Factor</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="25" t="inlineStr">
         <is>
           <t>Curtailment</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="25" t="inlineStr">
         <is>
           <t>Capital Expenditure</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="25" t="inlineStr">
         <is>
           <t>Operational Expenditure</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="25" t="inlineStr">
         <is>
           <t>Revenue</t>
         </is>
       </c>
-      <c r="N1" s="3" t="inlineStr">
+      <c r="N1" s="25" t="inlineStr">
         <is>
           <t>Market Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="24" t="inlineStr">
+      <c r="A2" s="26" t="inlineStr">
         <is>
           <t>Generator</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="25" t="inlineStr">
         <is>
           <t>solar</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>360.01739</v>
+        <v>343.52381</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>372614.17103</v>
+        <v>418320.1786639999</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>372614.17103</v>
+        <v>418320.1786639999</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1181494593913922</v>
+        <v>0.1390105828558668</v>
       </c>
       <c r="J2" t="n">
-        <v>225377.56069</v>
+        <v>152275.584260159</v>
       </c>
       <c r="K2" t="n">
-        <v>15282764.31072</v>
+        <v>16350630.95348142</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>15282764.19317</v>
+        <v>16350630.82707278</v>
       </c>
       <c r="N2" t="n">
-        <v>41.014987824391</v>
+        <v>39.08640238033033</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="n"/>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="A3" s="27" t="n"/>
+      <c r="B3" s="25" t="inlineStr">
         <is>
           <t>wind</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>696.83473</v>
+        <v>419.36757</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1563190.58011</v>
+        <v>1518065.943551292</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1563190.58011</v>
+        <v>1518065.943551292</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2560813953690281</v>
+        <v>0.413229852359677</v>
       </c>
       <c r="J3" t="n">
-        <v>1599117.20158</v>
+        <v>385067.2871604603</v>
       </c>
       <c r="K3" t="n">
-        <v>38225911.70514</v>
+        <v>27886858.4715285</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>38225911.6181</v>
+        <v>27886858.50362715</v>
       </c>
       <c r="N3" t="n">
-        <v>24.45377601039999</v>
+        <v>18.3699915159086</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24" t="inlineStr">
+      <c r="A4" s="26" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>Electrolyser</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>307.58628</v>
+        <v>282.08995</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1068290.76842</v>
+        <v>1068290.768400871</v>
       </c>
       <c r="F4" t="n">
-        <v>1810662.31936</v>
+        <v>1810662.319323497</v>
       </c>
       <c r="G4" t="n">
-        <v>-742371.55094</v>
+        <v>-742371.5509226257</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6719955454450049</v>
+        <v>0.7327329874563765</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>15931385.00964</v>
+        <v>24719667.0156932</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>15931385.01186</v>
+        <v>24719667.12472685</v>
       </c>
       <c r="N4" t="n">
-        <v>14.91296717534092</v>
+        <v>23.139455900878</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="20" t="n"/>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="A5" s="28" t="n"/>
+      <c r="B5" s="25" t="inlineStr">
         <is>
           <t>Haber-Bosch</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14.49032</v>
+        <v>130.89689</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>875999.97412</v>
+        <v>876000.0151150912</v>
       </c>
       <c r="F5" t="n">
-        <v>1192682.72477</v>
+        <v>1192682.780579355</v>
       </c>
       <c r="G5" t="n">
-        <v>-316682.75065</v>
+        <v>-316682.7654642642</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9799645556481844</v>
+        <v>0.9316569866879479</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>6329181.61895</v>
+        <v>9841556.480805896</v>
       </c>
       <c r="L5" t="n">
-        <v>9505475.71923</v>
+        <v>11592023.23677645</v>
       </c>
       <c r="M5" t="n">
-        <v>15834656.41937</v>
+        <v>21433579.80499268</v>
       </c>
       <c r="N5" t="n">
-        <v>18.0760918</v>
+        <v>24.46755643283428</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="n"/>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="A6" s="28" t="n"/>
+      <c r="B6" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>38.77327</v>
+        <v>35.598616</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>33109.60023</v>
+        <v>100991.2282849006</v>
       </c>
       <c r="F6" t="n">
-        <v>33109.60023</v>
+        <v>100991.2282849006</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00017</v>
+        <v>-0.0005952198591785418</v>
       </c>
       <c r="I6" t="n">
-        <v>0.09748030021713414</v>
+        <v>0.3238518887351305</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -6287,39 +6293,42 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0.00017</v>
+        <v>-0.0005952197495844302</v>
       </c>
       <c r="M6" t="n">
-        <v>0.00017</v>
+        <v>-0.000595280434936285</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-5.893316404424336e-09</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="n"/>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="A7" s="27" t="n"/>
+      <c r="B7" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>124.44434</v>
+        <v>130.89689</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>316366.22357</v>
+        <v>311401.7047741083</v>
       </c>
       <c r="F7" t="n">
-        <v>316366.22357</v>
+        <v>311401.7047741083</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00056</v>
+        <v>0.0009048259299220263</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2902090203539993</v>
+        <v>0.2715736012856838</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -6328,19 +6337,22 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00056</v>
+        <v>0.0009048259728956509</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00056</v>
+        <v>0.0009048543870449066</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2.905632640435153e-09</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="25" t="inlineStr">
         <is>
           <t>Load</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6373,156 +6385,156 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>-96503016.2263</v>
+        <v>-101123915.4402031</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="25" t="inlineStr">
         <is>
           <t>StorageUnit</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>35.48812</v>
+        <v>39.68199</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>10161.22664</v>
+        <v>18032.965364382</v>
       </c>
       <c r="F9" t="n">
-        <v>10911.67727</v>
+        <v>19364.77801297999</v>
       </c>
       <c r="G9" t="n">
-        <v>-750.45063</v>
+        <v>-1331.812648597994</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.06778550117616824</v>
+        <v>0.1075840396958441</v>
       </c>
       <c r="J9" t="n">
-        <v>311626.38183</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>654527.6693900001</v>
+        <v>816298.4602393163</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>654527.6666699999</v>
+        <v>816298.4578616484</v>
       </c>
       <c r="N9" t="n">
-        <v>64.41409186523673</v>
+        <v>45.26701190664786</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="24" t="inlineStr">
+      <c r="A10" s="26" t="inlineStr">
         <is>
           <t>Store</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="25" t="inlineStr">
         <is>
           <t>ammonia</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7598.3423</v>
+        <v>27648.721</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>16554.80003</v>
+        <v>50495.61444005983</v>
       </c>
       <c r="F10" t="n">
-        <v>16554.8002</v>
+        <v>50495.61384484063</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.00017</v>
+        <v>0.0005952198591785418</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3408220185079053</v>
+        <v>0.4128602762794727</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>73221.59957999999</v>
+        <v>3149969.023766937</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.00017</v>
+        <v>0.0005952198591785418</v>
       </c>
       <c r="M10" t="n">
-        <v>73221.58136</v>
+        <v>3149969.084919804</v>
       </c>
       <c r="N10" t="n">
-        <v>4.422976791440455</v>
+        <v>62.38104278657743</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="n"/>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="A11" s="27" t="n"/>
+      <c r="B11" s="25" t="inlineStr">
         <is>
           <t>hydrogen</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2070.5468</v>
+        <v>4229.545</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>158183.11151</v>
+        <v>155700.851934641</v>
       </c>
       <c r="F11" t="n">
-        <v>158183.11206</v>
+        <v>155700.8528394664</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.00056</v>
+        <v>-0.0009048259283304105</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1405904324403583</v>
+        <v>0.2748945924757951</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>10500548.03347</v>
+        <v>6766913.169922759</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.00056</v>
+        <v>-0.0009048259283304105</v>
       </c>
       <c r="M11" t="n">
-        <v>10500548.23495</v>
+        <v>6766912.919244</v>
       </c>
       <c r="N11" t="n">
-        <v>66.38224376337054</v>
+        <v>43.46098839641905</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="25" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="25" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -6535,7 +6547,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>875999.97412</v>
+        <v>876000.0151150912</v>
       </c>
     </row>
     <row r="16">
@@ -6545,7 +6557,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>86997539.94689001</v>
+        <v>89531893.57543801</v>
       </c>
     </row>
     <row r="17">
@@ -6555,7 +6567,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9505475.71923</v>
+        <v>11592023.23677645</v>
       </c>
     </row>
     <row r="18">
@@ -6565,7 +6577,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>572.8489683666157</v>
+        <v>600.2789478884066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>